<commit_message>
audio list 1 added
</commit_message>
<xml_diff>
--- a/resources/list2.xlsx
+++ b/resources/list2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marie\Desktop\Experiment Neurolinguïstiek\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4118262A-BEC4-47A1-A447-4E67DF0D782E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A253149-CDB5-4278-A4CA-E2EDE79538DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -2148,13 +2148,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="Q64" sqref="Q64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="4" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" bestFit="1" customWidth="1"/>

</xml_diff>